<commit_message>
Finalizing Phase 2 Stock Criteria
</commit_message>
<xml_diff>
--- a/CoreExcelFiles/P2MasterTemplate5.27.23.xlsx
+++ b/CoreExcelFiles/P2MasterTemplate5.27.23.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Lucas\AI Picker 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Automated-Stock-Selector\CoreExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D761B6-BFA1-44C2-A2C1-EF0D26DAFC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AFA31C-5330-4746-9032-89EBAC8E66F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="896" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="896" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Industrials" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Finance" sheetId="11" r:id="rId11"/>
     <sheet name="Basic Materials" sheetId="12" r:id="rId12"/>
     <sheet name="Unspecified" sheetId="13" r:id="rId13"/>
-    <sheet name="FAILS" sheetId="14" r:id="rId14"/>
+    <sheet name="ELIMINATED" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="55">
   <si>
     <t>Company Name</t>
   </si>
@@ -190,6 +190,27 @@
   </si>
   <si>
     <t>Industry</t>
+  </si>
+  <si>
+    <t>Curr. Price</t>
+  </si>
+  <si>
+    <t>52 High</t>
+  </si>
+  <si>
+    <t>52 Low</t>
+  </si>
+  <si>
+    <t>Reason for Elimination</t>
+  </si>
+  <si>
+    <t>TTM</t>
+  </si>
+  <si>
+    <t>High (Series 2)</t>
+  </si>
+  <si>
+    <t>Low (Series 2)</t>
   </si>
 </sst>
 </file>
@@ -246,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -292,11 +313,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -325,6 +357,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1563,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AO2"/>
+  <dimension ref="A1:CG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BD17" sqref="BD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1577,44 +1620,38 @@
     <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="33" width="6.77734375" customWidth="1"/>
+    <col min="34" max="34" width="6.77734375" style="2" customWidth="1"/>
+    <col min="35" max="51" width="6.77734375" customWidth="1"/>
+    <col min="52" max="52" width="6.77734375" style="2" customWidth="1"/>
+    <col min="53" max="53" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="68" max="85" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -1625,7 +1662,7 @@
       <c r="F1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -1634,38 +1671,65 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
       <c r="AH1" s="10"/>
       <c r="AI1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="14"/>
+      <c r="BH1" s="14"/>
+      <c r="BI1" s="15"/>
+      <c r="BJ1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
     </row>
-    <row r="2" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:85" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1682,120 +1746,250 @@
         <v>32</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="3" t="s">
+      <c r="Q2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="3">
+        <v>2023</v>
+      </c>
+      <c r="S2" s="3">
+        <v>2022</v>
+      </c>
+      <c r="T2" s="3">
+        <v>2021</v>
+      </c>
+      <c r="U2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="V2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="W2" s="3">
+        <v>2018</v>
+      </c>
+      <c r="X2" s="3">
+        <v>2017</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>2016</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>2015</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>2014</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>2013</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>2012</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>2011</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>2010</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>2009</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>2008</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>2007</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>2023</v>
+      </c>
+      <c r="AK2" s="3">
+        <v>2022</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>2021</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="AN2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>2018</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>2017</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>2016</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>2015</v>
+      </c>
+      <c r="AS2" s="3">
+        <v>2014</v>
+      </c>
+      <c r="AT2" s="3">
+        <v>2013</v>
+      </c>
+      <c r="AU2" s="3">
+        <v>2012</v>
+      </c>
+      <c r="AV2" s="3">
+        <v>2011</v>
+      </c>
+      <c r="AW2" s="3">
+        <v>2010</v>
+      </c>
+      <c r="AX2" s="3">
+        <v>2009</v>
+      </c>
+      <c r="AY2" s="3">
+        <v>2008</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>2007</v>
+      </c>
+      <c r="BA2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="BE2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="BF2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="BG2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="BH2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH2" s="4" t="s">
+      <c r="BI2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="BK2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="BL2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN2" s="3" t="s">
+      <c r="BM2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="BN2" s="3" t="s">
         <v>43</v>
+      </c>
+      <c r="BP2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="BQ2" s="3">
+        <v>2023</v>
+      </c>
+      <c r="BR2" s="3">
+        <v>2022</v>
+      </c>
+      <c r="BS2" s="3">
+        <v>2021</v>
+      </c>
+      <c r="BT2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="BU2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="BV2" s="3">
+        <v>2018</v>
+      </c>
+      <c r="BW2" s="3">
+        <v>2017</v>
+      </c>
+      <c r="BX2" s="3">
+        <v>2016</v>
+      </c>
+      <c r="BY2" s="3">
+        <v>2015</v>
+      </c>
+      <c r="BZ2" s="3">
+        <v>2014</v>
+      </c>
+      <c r="CA2" s="3">
+        <v>2013</v>
+      </c>
+      <c r="CB2" s="3">
+        <v>2012</v>
+      </c>
+      <c r="CC2" s="3">
+        <v>2011</v>
+      </c>
+      <c r="CD2" s="3">
+        <v>2010</v>
+      </c>
+      <c r="CE2" s="3">
+        <v>2009</v>
+      </c>
+      <c r="CF2" s="3">
+        <v>2008</v>
+      </c>
+      <c r="CG2" s="3">
+        <v>2007</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F1:Q1"/>
+  <mergeCells count="5">
+    <mergeCell ref="F1:P1"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="R1:AH1"/>
-    <mergeCell ref="AI1:AO1"/>
+    <mergeCell ref="BJ1:BN1"/>
+    <mergeCell ref="Q1:AH1"/>
+    <mergeCell ref="AI1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1804,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224FA0DE-C4B9-4BF5-B9F4-23F7496C55BD}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,9 +2009,10 @@
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="60.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>45</v>
       </c>
@@ -1835,6 +2030,9 @@
       </c>
       <c r="F1" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>